<commit_message>
gitignore is now working
</commit_message>
<xml_diff>
--- a/Data/Odds/NBA/NBA odds 2021-22.xlsx
+++ b/Data/Odds/NBA/NBA odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M637"/>
+  <dimension ref="A1:M725"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29170,6 +29170,3968 @@
         <v>1</v>
       </c>
     </row>
+    <row r="638">
+      <c r="A638" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B638" t="n">
+        <v>539</v>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E638" t="n">
+        <v>24</v>
+      </c>
+      <c r="F638" t="n">
+        <v>33</v>
+      </c>
+      <c r="G638" t="n">
+        <v>31</v>
+      </c>
+      <c r="H638" t="n">
+        <v>19</v>
+      </c>
+      <c r="I638" t="n">
+        <v>107</v>
+      </c>
+      <c r="J638" t="n">
+        <v>216.5</v>
+      </c>
+      <c r="K638" t="n">
+        <v>217</v>
+      </c>
+      <c r="L638" t="n">
+        <v>150</v>
+      </c>
+      <c r="M638" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B639" t="n">
+        <v>540</v>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E639" t="n">
+        <v>24</v>
+      </c>
+      <c r="F639" t="n">
+        <v>29</v>
+      </c>
+      <c r="G639" t="n">
+        <v>38</v>
+      </c>
+      <c r="H639" t="n">
+        <v>24</v>
+      </c>
+      <c r="I639" t="n">
+        <v>115</v>
+      </c>
+      <c r="J639" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K639" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L639" t="n">
+        <v>-170</v>
+      </c>
+      <c r="M639" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B640" t="n">
+        <v>541</v>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E640" t="n">
+        <v>38</v>
+      </c>
+      <c r="F640" t="n">
+        <v>27</v>
+      </c>
+      <c r="G640" t="n">
+        <v>22</v>
+      </c>
+      <c r="H640" t="n">
+        <v>27</v>
+      </c>
+      <c r="I640" t="n">
+        <v>114</v>
+      </c>
+      <c r="J640" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="K640" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="L640" t="n">
+        <v>115</v>
+      </c>
+      <c r="M640" t="n">
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B641" t="n">
+        <v>542</v>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="E641" t="n">
+        <v>29</v>
+      </c>
+      <c r="F641" t="n">
+        <v>28</v>
+      </c>
+      <c r="G641" t="n">
+        <v>31</v>
+      </c>
+      <c r="H641" t="n">
+        <v>23</v>
+      </c>
+      <c r="I641" t="n">
+        <v>111</v>
+      </c>
+      <c r="J641" t="n">
+        <v>1</v>
+      </c>
+      <c r="K641" t="n">
+        <v>2</v>
+      </c>
+      <c r="L641" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M641" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B642" t="n">
+        <v>543</v>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E642" t="n">
+        <v>29</v>
+      </c>
+      <c r="F642" t="n">
+        <v>34</v>
+      </c>
+      <c r="G642" t="n">
+        <v>20</v>
+      </c>
+      <c r="H642" t="n">
+        <v>20</v>
+      </c>
+      <c r="I642" t="n">
+        <v>103</v>
+      </c>
+      <c r="J642" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K642" t="n">
+        <v>8</v>
+      </c>
+      <c r="L642" t="n">
+        <v>-340</v>
+      </c>
+      <c r="M642" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B643" t="n">
+        <v>544</v>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="E643" t="n">
+        <v>15</v>
+      </c>
+      <c r="F643" t="n">
+        <v>32</v>
+      </c>
+      <c r="G643" t="n">
+        <v>32</v>
+      </c>
+      <c r="H643" t="n">
+        <v>29</v>
+      </c>
+      <c r="I643" t="n">
+        <v>108</v>
+      </c>
+      <c r="J643" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="K643" t="n">
+        <v>208</v>
+      </c>
+      <c r="L643" t="n">
+        <v>280</v>
+      </c>
+      <c r="M643" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B644" t="n">
+        <v>545</v>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E644" t="n">
+        <v>20</v>
+      </c>
+      <c r="F644" t="n">
+        <v>20</v>
+      </c>
+      <c r="G644" t="n">
+        <v>23</v>
+      </c>
+      <c r="H644" t="n">
+        <v>24</v>
+      </c>
+      <c r="I644" t="n">
+        <v>87</v>
+      </c>
+      <c r="J644" t="n">
+        <v>210.5</v>
+      </c>
+      <c r="K644" t="n">
+        <v>206.5</v>
+      </c>
+      <c r="L644" t="n">
+        <v>135</v>
+      </c>
+      <c r="M644" t="n">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B645" t="n">
+        <v>546</v>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="E645" t="n">
+        <v>21</v>
+      </c>
+      <c r="F645" t="n">
+        <v>23</v>
+      </c>
+      <c r="G645" t="n">
+        <v>20</v>
+      </c>
+      <c r="H645" t="n">
+        <v>24</v>
+      </c>
+      <c r="I645" t="n">
+        <v>88</v>
+      </c>
+      <c r="J645" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K645" t="n">
+        <v>3</v>
+      </c>
+      <c r="L645" t="n">
+        <v>-155</v>
+      </c>
+      <c r="M645" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B646" t="n">
+        <v>547</v>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E646" t="n">
+        <v>31</v>
+      </c>
+      <c r="F646" t="n">
+        <v>30</v>
+      </c>
+      <c r="G646" t="n">
+        <v>26</v>
+      </c>
+      <c r="H646" t="n">
+        <v>24</v>
+      </c>
+      <c r="I646" t="n">
+        <v>111</v>
+      </c>
+      <c r="J646" t="n">
+        <v>204.5</v>
+      </c>
+      <c r="K646" t="n">
+        <v>206.5</v>
+      </c>
+      <c r="L646" t="n">
+        <v>130</v>
+      </c>
+      <c r="M646" t="n">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B647" t="n">
+        <v>548</v>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E647" t="n">
+        <v>16</v>
+      </c>
+      <c r="F647" t="n">
+        <v>27</v>
+      </c>
+      <c r="G647" t="n">
+        <v>20</v>
+      </c>
+      <c r="H647" t="n">
+        <v>22</v>
+      </c>
+      <c r="I647" t="n">
+        <v>85</v>
+      </c>
+      <c r="J647" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K647" t="n">
+        <v>3</v>
+      </c>
+      <c r="L647" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M647" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B648" t="n">
+        <v>549</v>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E648" t="n">
+        <v>41</v>
+      </c>
+      <c r="F648" t="n">
+        <v>26</v>
+      </c>
+      <c r="G648" t="n">
+        <v>35</v>
+      </c>
+      <c r="H648" t="n">
+        <v>37</v>
+      </c>
+      <c r="I648" t="n">
+        <v>139</v>
+      </c>
+      <c r="J648" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K648" t="n">
+        <v>4</v>
+      </c>
+      <c r="L648" t="n">
+        <v>-170</v>
+      </c>
+      <c r="M648" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B649" t="n">
+        <v>550</v>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E649" t="n">
+        <v>23</v>
+      </c>
+      <c r="F649" t="n">
+        <v>23</v>
+      </c>
+      <c r="G649" t="n">
+        <v>29</v>
+      </c>
+      <c r="H649" t="n">
+        <v>32</v>
+      </c>
+      <c r="I649" t="n">
+        <v>107</v>
+      </c>
+      <c r="J649" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="K649" t="n">
+        <v>216</v>
+      </c>
+      <c r="L649" t="n">
+        <v>150</v>
+      </c>
+      <c r="M649" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B650" t="n">
+        <v>551</v>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E650" t="n">
+        <v>24</v>
+      </c>
+      <c r="F650" t="n">
+        <v>29</v>
+      </c>
+      <c r="G650" t="n">
+        <v>20</v>
+      </c>
+      <c r="H650" t="n">
+        <v>41</v>
+      </c>
+      <c r="I650" t="n">
+        <v>114</v>
+      </c>
+      <c r="J650" t="n">
+        <v>211.5</v>
+      </c>
+      <c r="K650" t="n">
+        <v>216.5</v>
+      </c>
+      <c r="L650" t="n">
+        <v>115</v>
+      </c>
+      <c r="M650" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B651" t="n">
+        <v>552</v>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>OklahomaCity</t>
+        </is>
+      </c>
+      <c r="E651" t="n">
+        <v>26</v>
+      </c>
+      <c r="F651" t="n">
+        <v>34</v>
+      </c>
+      <c r="G651" t="n">
+        <v>21</v>
+      </c>
+      <c r="H651" t="n">
+        <v>29</v>
+      </c>
+      <c r="I651" t="n">
+        <v>110</v>
+      </c>
+      <c r="J651" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K651" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L651" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M651" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B652" t="n">
+        <v>553</v>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="E652" t="n">
+        <v>41</v>
+      </c>
+      <c r="F652" t="n">
+        <v>27</v>
+      </c>
+      <c r="G652" t="n">
+        <v>27</v>
+      </c>
+      <c r="H652" t="n">
+        <v>30</v>
+      </c>
+      <c r="I652" t="n">
+        <v>125</v>
+      </c>
+      <c r="J652" t="n">
+        <v>230</v>
+      </c>
+      <c r="K652" t="n">
+        <v>230.5</v>
+      </c>
+      <c r="L652" t="n">
+        <v>300</v>
+      </c>
+      <c r="M652" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B653" t="n">
+        <v>554</v>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E653" t="n">
+        <v>25</v>
+      </c>
+      <c r="F653" t="n">
+        <v>35</v>
+      </c>
+      <c r="G653" t="n">
+        <v>37</v>
+      </c>
+      <c r="H653" t="n">
+        <v>30</v>
+      </c>
+      <c r="I653" t="n">
+        <v>127</v>
+      </c>
+      <c r="J653" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K653" t="n">
+        <v>9</v>
+      </c>
+      <c r="L653" t="n">
+        <v>-360</v>
+      </c>
+      <c r="M653" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B654" t="n">
+        <v>555</v>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>Sacramento</t>
+        </is>
+      </c>
+      <c r="E654" t="n">
+        <v>29</v>
+      </c>
+      <c r="F654" t="n">
+        <v>33</v>
+      </c>
+      <c r="G654" t="n">
+        <v>37</v>
+      </c>
+      <c r="H654" t="n">
+        <v>25</v>
+      </c>
+      <c r="I654" t="n">
+        <v>124</v>
+      </c>
+      <c r="J654" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K654" t="n">
+        <v>215</v>
+      </c>
+      <c r="L654" t="n">
+        <v>205</v>
+      </c>
+      <c r="M654" t="n">
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="n">
+        <v>1201</v>
+      </c>
+      <c r="B655" t="n">
+        <v>556</v>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E655" t="n">
+        <v>21</v>
+      </c>
+      <c r="F655" t="n">
+        <v>31</v>
+      </c>
+      <c r="G655" t="n">
+        <v>24</v>
+      </c>
+      <c r="H655" t="n">
+        <v>39</v>
+      </c>
+      <c r="I655" t="n">
+        <v>115</v>
+      </c>
+      <c r="J655" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K655" t="n">
+        <v>6</v>
+      </c>
+      <c r="L655" t="n">
+        <v>-245</v>
+      </c>
+      <c r="M655" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B656" t="n">
+        <v>557</v>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E656" t="n">
+        <v>37</v>
+      </c>
+      <c r="F656" t="n">
+        <v>32</v>
+      </c>
+      <c r="G656" t="n">
+        <v>20</v>
+      </c>
+      <c r="H656" t="n">
+        <v>30</v>
+      </c>
+      <c r="I656" t="n">
+        <v>119</v>
+      </c>
+      <c r="J656" t="n">
+        <v>1</v>
+      </c>
+      <c r="K656" t="n">
+        <v>2</v>
+      </c>
+      <c r="L656" t="n">
+        <v>-115</v>
+      </c>
+      <c r="M656" t="n">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B657" t="n">
+        <v>558</v>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>NewYork</t>
+        </is>
+      </c>
+      <c r="E657" t="n">
+        <v>19</v>
+      </c>
+      <c r="F657" t="n">
+        <v>32</v>
+      </c>
+      <c r="G657" t="n">
+        <v>32</v>
+      </c>
+      <c r="H657" t="n">
+        <v>32</v>
+      </c>
+      <c r="I657" t="n">
+        <v>115</v>
+      </c>
+      <c r="J657" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="K657" t="n">
+        <v>209.5</v>
+      </c>
+      <c r="L657" t="n">
+        <v>-105</v>
+      </c>
+      <c r="M657" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B658" t="n">
+        <v>559</v>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E658" t="n">
+        <v>23</v>
+      </c>
+      <c r="F658" t="n">
+        <v>17</v>
+      </c>
+      <c r="G658" t="n">
+        <v>28</v>
+      </c>
+      <c r="H658" t="n">
+        <v>25</v>
+      </c>
+      <c r="I658" t="n">
+        <v>93</v>
+      </c>
+      <c r="J658" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K658" t="n">
+        <v>216</v>
+      </c>
+      <c r="L658" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M658" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B659" t="n">
+        <v>560</v>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>Toronto</t>
+        </is>
+      </c>
+      <c r="E659" t="n">
+        <v>26</v>
+      </c>
+      <c r="F659" t="n">
+        <v>22</v>
+      </c>
+      <c r="G659" t="n">
+        <v>25</v>
+      </c>
+      <c r="H659" t="n">
+        <v>24</v>
+      </c>
+      <c r="I659" t="n">
+        <v>97</v>
+      </c>
+      <c r="J659" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="K659" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L659" t="n">
+        <v>130</v>
+      </c>
+      <c r="M659" t="n">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B660" t="n">
+        <v>561</v>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>OklahomaCity</t>
+        </is>
+      </c>
+      <c r="E660" t="n">
+        <v>16</v>
+      </c>
+      <c r="F660" t="n">
+        <v>20</v>
+      </c>
+      <c r="G660" t="n">
+        <v>26</v>
+      </c>
+      <c r="H660" t="n">
+        <v>17</v>
+      </c>
+      <c r="I660" t="n">
+        <v>79</v>
+      </c>
+      <c r="J660" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K660" t="n">
+        <v>210.5</v>
+      </c>
+      <c r="L660" t="n">
+        <v>340</v>
+      </c>
+      <c r="M660" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B661" t="n">
+        <v>562</v>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>Memphis</t>
+        </is>
+      </c>
+      <c r="E661" t="n">
+        <v>31</v>
+      </c>
+      <c r="F661" t="n">
+        <v>41</v>
+      </c>
+      <c r="G661" t="n">
+        <v>41</v>
+      </c>
+      <c r="H661" t="n">
+        <v>39</v>
+      </c>
+      <c r="I661" t="n">
+        <v>152</v>
+      </c>
+      <c r="J661" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K661" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="L661" t="n">
+        <v>-430</v>
+      </c>
+      <c r="M661" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B662" t="n">
+        <v>563</v>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E662" t="n">
+        <v>18</v>
+      </c>
+      <c r="F662" t="n">
+        <v>33</v>
+      </c>
+      <c r="G662" t="n">
+        <v>30</v>
+      </c>
+      <c r="H662" t="n">
+        <v>22</v>
+      </c>
+      <c r="I662" t="n">
+        <v>103</v>
+      </c>
+      <c r="J662" t="n">
+        <v>210.5</v>
+      </c>
+      <c r="K662" t="n">
+        <v>208</v>
+      </c>
+      <c r="L662" t="n">
+        <v>700</v>
+      </c>
+      <c r="M662" t="n">
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B663" t="n">
+        <v>564</v>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E663" t="n">
+        <v>30</v>
+      </c>
+      <c r="F663" t="n">
+        <v>39</v>
+      </c>
+      <c r="G663" t="n">
+        <v>18</v>
+      </c>
+      <c r="H663" t="n">
+        <v>27</v>
+      </c>
+      <c r="I663" t="n">
+        <v>114</v>
+      </c>
+      <c r="J663" t="n">
+        <v>13</v>
+      </c>
+      <c r="K663" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="L663" t="n">
+        <v>-1100</v>
+      </c>
+      <c r="M663" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B664" t="n">
+        <v>565</v>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>SanAntonio</t>
+        </is>
+      </c>
+      <c r="E664" t="n">
+        <v>32</v>
+      </c>
+      <c r="F664" t="n">
+        <v>36</v>
+      </c>
+      <c r="G664" t="n">
+        <v>16</v>
+      </c>
+      <c r="H664" t="n">
+        <v>30</v>
+      </c>
+      <c r="I664" t="n">
+        <v>114</v>
+      </c>
+      <c r="J664" t="n">
+        <v>221.5</v>
+      </c>
+      <c r="K664" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="L664" t="n">
+        <v>195</v>
+      </c>
+      <c r="M664" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="n">
+        <v>1202</v>
+      </c>
+      <c r="B665" t="n">
+        <v>566</v>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>Portland</t>
+        </is>
+      </c>
+      <c r="E665" t="n">
+        <v>22</v>
+      </c>
+      <c r="F665" t="n">
+        <v>25</v>
+      </c>
+      <c r="G665" t="n">
+        <v>18</v>
+      </c>
+      <c r="H665" t="n">
+        <v>18</v>
+      </c>
+      <c r="I665" t="n">
+        <v>83</v>
+      </c>
+      <c r="J665" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K665" t="n">
+        <v>5</v>
+      </c>
+      <c r="L665" t="n">
+        <v>-230</v>
+      </c>
+      <c r="M665" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B666" t="n">
+        <v>501</v>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E666" t="n">
+        <v>32</v>
+      </c>
+      <c r="F666" t="n">
+        <v>30</v>
+      </c>
+      <c r="G666" t="n">
+        <v>30</v>
+      </c>
+      <c r="H666" t="n">
+        <v>21</v>
+      </c>
+      <c r="I666" t="n">
+        <v>113</v>
+      </c>
+      <c r="J666" t="n">
+        <v>208</v>
+      </c>
+      <c r="K666" t="n">
+        <v>206</v>
+      </c>
+      <c r="L666" t="n">
+        <v>190</v>
+      </c>
+      <c r="M666" t="n">
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B667" t="n">
+        <v>502</v>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="E667" t="n">
+        <v>25</v>
+      </c>
+      <c r="F667" t="n">
+        <v>30</v>
+      </c>
+      <c r="G667" t="n">
+        <v>26</v>
+      </c>
+      <c r="H667" t="n">
+        <v>23</v>
+      </c>
+      <c r="I667" t="n">
+        <v>104</v>
+      </c>
+      <c r="J667" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K667" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L667" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M667" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B668" t="n">
+        <v>503</v>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E668" t="n">
+        <v>34</v>
+      </c>
+      <c r="F668" t="n">
+        <v>31</v>
+      </c>
+      <c r="G668" t="n">
+        <v>34</v>
+      </c>
+      <c r="H668" t="n">
+        <v>17</v>
+      </c>
+      <c r="I668" t="n">
+        <v>116</v>
+      </c>
+      <c r="J668" t="n">
+        <v>209</v>
+      </c>
+      <c r="K668" t="n">
+        <v>208.5</v>
+      </c>
+      <c r="L668" t="n">
+        <v>130</v>
+      </c>
+      <c r="M668" t="n">
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B669" t="n">
+        <v>504</v>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E669" t="n">
+        <v>29</v>
+      </c>
+      <c r="F669" t="n">
+        <v>17</v>
+      </c>
+      <c r="G669" t="n">
+        <v>26</v>
+      </c>
+      <c r="H669" t="n">
+        <v>29</v>
+      </c>
+      <c r="I669" t="n">
+        <v>101</v>
+      </c>
+      <c r="J669" t="n">
+        <v>3</v>
+      </c>
+      <c r="K669" t="n">
+        <v>3</v>
+      </c>
+      <c r="L669" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M669" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B670" t="n">
+        <v>505</v>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E670" t="n">
+        <v>31</v>
+      </c>
+      <c r="F670" t="n">
+        <v>13</v>
+      </c>
+      <c r="G670" t="n">
+        <v>34</v>
+      </c>
+      <c r="H670" t="n">
+        <v>20</v>
+      </c>
+      <c r="I670" t="n">
+        <v>98</v>
+      </c>
+      <c r="J670" t="n">
+        <v>213</v>
+      </c>
+      <c r="K670" t="n">
+        <v>216</v>
+      </c>
+      <c r="L670" t="n">
+        <v>120</v>
+      </c>
+      <c r="M670" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B671" t="n">
+        <v>506</v>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E671" t="n">
+        <v>22</v>
+      </c>
+      <c r="F671" t="n">
+        <v>30</v>
+      </c>
+      <c r="G671" t="n">
+        <v>35</v>
+      </c>
+      <c r="H671" t="n">
+        <v>9</v>
+      </c>
+      <c r="I671" t="n">
+        <v>96</v>
+      </c>
+      <c r="J671" t="n">
+        <v>3</v>
+      </c>
+      <c r="K671" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L671" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M671" t="n">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B672" t="n">
+        <v>507</v>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E672" t="n">
+        <v>34</v>
+      </c>
+      <c r="F672" t="n">
+        <v>21</v>
+      </c>
+      <c r="G672" t="n">
+        <v>30</v>
+      </c>
+      <c r="H672" t="n">
+        <v>20</v>
+      </c>
+      <c r="I672" t="n">
+        <v>105</v>
+      </c>
+      <c r="J672" t="n">
+        <v>219</v>
+      </c>
+      <c r="K672" t="n">
+        <v>219</v>
+      </c>
+      <c r="L672" t="n">
+        <v>340</v>
+      </c>
+      <c r="M672" t="n">
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B673" t="n">
+        <v>508</v>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E673" t="n">
+        <v>27</v>
+      </c>
+      <c r="F673" t="n">
+        <v>32</v>
+      </c>
+      <c r="G673" t="n">
+        <v>27</v>
+      </c>
+      <c r="H673" t="n">
+        <v>24</v>
+      </c>
+      <c r="I673" t="n">
+        <v>110</v>
+      </c>
+      <c r="J673" t="n">
+        <v>8</v>
+      </c>
+      <c r="K673" t="n">
+        <v>9</v>
+      </c>
+      <c r="L673" t="n">
+        <v>-410</v>
+      </c>
+      <c r="M673" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B674" t="n">
+        <v>509</v>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="E674" t="n">
+        <v>24</v>
+      </c>
+      <c r="F674" t="n">
+        <v>32</v>
+      </c>
+      <c r="G674" t="n">
+        <v>27</v>
+      </c>
+      <c r="H674" t="n">
+        <v>33</v>
+      </c>
+      <c r="I674" t="n">
+        <v>116</v>
+      </c>
+      <c r="J674" t="n">
+        <v>216</v>
+      </c>
+      <c r="K674" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="L674" t="n">
+        <v>130</v>
+      </c>
+      <c r="M674" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B675" t="n">
+        <v>510</v>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E675" t="n">
+        <v>31</v>
+      </c>
+      <c r="F675" t="n">
+        <v>23</v>
+      </c>
+      <c r="G675" t="n">
+        <v>30</v>
+      </c>
+      <c r="H675" t="n">
+        <v>34</v>
+      </c>
+      <c r="I675" t="n">
+        <v>118</v>
+      </c>
+      <c r="J675" t="n">
+        <v>3</v>
+      </c>
+      <c r="K675" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L675" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M675" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B676" t="n">
+        <v>511</v>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E676" t="n">
+        <v>14</v>
+      </c>
+      <c r="F676" t="n">
+        <v>30</v>
+      </c>
+      <c r="G676" t="n">
+        <v>35</v>
+      </c>
+      <c r="H676" t="n">
+        <v>28</v>
+      </c>
+      <c r="I676" t="n">
+        <v>107</v>
+      </c>
+      <c r="J676" t="n">
+        <v>218.5</v>
+      </c>
+      <c r="K676" t="n">
+        <v>215</v>
+      </c>
+      <c r="L676" t="n">
+        <v>250</v>
+      </c>
+      <c r="M676" t="n">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B677" t="n">
+        <v>512</v>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E677" t="n">
+        <v>19</v>
+      </c>
+      <c r="F677" t="n">
+        <v>29</v>
+      </c>
+      <c r="G677" t="n">
+        <v>20</v>
+      </c>
+      <c r="H677" t="n">
+        <v>23</v>
+      </c>
+      <c r="I677" t="n">
+        <v>91</v>
+      </c>
+      <c r="J677" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K677" t="n">
+        <v>7</v>
+      </c>
+      <c r="L677" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M677" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B678" t="n">
+        <v>513</v>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="E678" t="n">
+        <v>25</v>
+      </c>
+      <c r="F678" t="n">
+        <v>31</v>
+      </c>
+      <c r="G678" t="n">
+        <v>41</v>
+      </c>
+      <c r="H678" t="n">
+        <v>33</v>
+      </c>
+      <c r="I678" t="n">
+        <v>130</v>
+      </c>
+      <c r="J678" t="n">
+        <v>213</v>
+      </c>
+      <c r="K678" t="n">
+        <v>209.5</v>
+      </c>
+      <c r="L678" t="n">
+        <v>290</v>
+      </c>
+      <c r="M678" t="n">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B679" t="n">
+        <v>514</v>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E679" t="n">
+        <v>38</v>
+      </c>
+      <c r="F679" t="n">
+        <v>21</v>
+      </c>
+      <c r="G679" t="n">
+        <v>41</v>
+      </c>
+      <c r="H679" t="n">
+        <v>37</v>
+      </c>
+      <c r="I679" t="n">
+        <v>137</v>
+      </c>
+      <c r="J679" t="n">
+        <v>9</v>
+      </c>
+      <c r="K679" t="n">
+        <v>8</v>
+      </c>
+      <c r="L679" t="n">
+        <v>-350</v>
+      </c>
+      <c r="M679" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B680" t="n">
+        <v>515</v>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E680" t="n">
+        <v>21</v>
+      </c>
+      <c r="F680" t="n">
+        <v>27</v>
+      </c>
+      <c r="G680" t="n">
+        <v>20</v>
+      </c>
+      <c r="H680" t="n">
+        <v>28</v>
+      </c>
+      <c r="I680" t="n">
+        <v>96</v>
+      </c>
+      <c r="J680" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K680" t="n">
+        <v>215</v>
+      </c>
+      <c r="L680" t="n">
+        <v>250</v>
+      </c>
+      <c r="M680" t="n">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B681" t="n">
+        <v>516</v>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>GoldenState</t>
+        </is>
+      </c>
+      <c r="E681" t="n">
+        <v>28</v>
+      </c>
+      <c r="F681" t="n">
+        <v>23</v>
+      </c>
+      <c r="G681" t="n">
+        <v>29</v>
+      </c>
+      <c r="H681" t="n">
+        <v>38</v>
+      </c>
+      <c r="I681" t="n">
+        <v>118</v>
+      </c>
+      <c r="J681" t="n">
+        <v>7</v>
+      </c>
+      <c r="K681" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L681" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M681" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B682" t="n">
+        <v>517</v>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E682" t="n">
+        <v>23</v>
+      </c>
+      <c r="F682" t="n">
+        <v>30</v>
+      </c>
+      <c r="G682" t="n">
+        <v>34</v>
+      </c>
+      <c r="H682" t="n">
+        <v>32</v>
+      </c>
+      <c r="I682" t="n">
+        <v>119</v>
+      </c>
+      <c r="J682" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K682" t="n">
+        <v>219</v>
+      </c>
+      <c r="L682" t="n">
+        <v>115</v>
+      </c>
+      <c r="M682" t="n">
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B683" t="n">
+        <v>518</v>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>LALakers</t>
+        </is>
+      </c>
+      <c r="E683" t="n">
+        <v>22</v>
+      </c>
+      <c r="F683" t="n">
+        <v>28</v>
+      </c>
+      <c r="G683" t="n">
+        <v>29</v>
+      </c>
+      <c r="H683" t="n">
+        <v>36</v>
+      </c>
+      <c r="I683" t="n">
+        <v>115</v>
+      </c>
+      <c r="J683" t="n">
+        <v>217</v>
+      </c>
+      <c r="K683" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L683" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M683" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B684" t="n">
+        <v>519</v>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E684" t="n">
+        <v>30</v>
+      </c>
+      <c r="F684" t="n">
+        <v>30</v>
+      </c>
+      <c r="G684" t="n">
+        <v>32</v>
+      </c>
+      <c r="H684" t="n">
+        <v>21</v>
+      </c>
+      <c r="I684" t="n">
+        <v>113</v>
+      </c>
+      <c r="J684" t="n">
+        <v>210.5</v>
+      </c>
+      <c r="K684" t="n">
+        <v>209</v>
+      </c>
+      <c r="L684" t="n">
+        <v>120</v>
+      </c>
+      <c r="M684" t="n">
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B685" t="n">
+        <v>520</v>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>NewYork</t>
+        </is>
+      </c>
+      <c r="E685" t="n">
+        <v>25</v>
+      </c>
+      <c r="F685" t="n">
+        <v>24</v>
+      </c>
+      <c r="G685" t="n">
+        <v>22</v>
+      </c>
+      <c r="H685" t="n">
+        <v>28</v>
+      </c>
+      <c r="I685" t="n">
+        <v>99</v>
+      </c>
+      <c r="J685" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K685" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L685" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M685" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B686" t="n">
+        <v>521</v>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E686" t="n">
+        <v>28</v>
+      </c>
+      <c r="F686" t="n">
+        <v>24</v>
+      </c>
+      <c r="G686" t="n">
+        <v>27</v>
+      </c>
+      <c r="H686" t="n">
+        <v>32</v>
+      </c>
+      <c r="I686" t="n">
+        <v>111</v>
+      </c>
+      <c r="J686" t="n">
+        <v>220</v>
+      </c>
+      <c r="K686" t="n">
+        <v>222</v>
+      </c>
+      <c r="L686" t="n">
+        <v>120</v>
+      </c>
+      <c r="M686" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B687" t="n">
+        <v>522</v>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>Brooklyn</t>
+        </is>
+      </c>
+      <c r="E687" t="n">
+        <v>34</v>
+      </c>
+      <c r="F687" t="n">
+        <v>22</v>
+      </c>
+      <c r="G687" t="n">
+        <v>26</v>
+      </c>
+      <c r="H687" t="n">
+        <v>25</v>
+      </c>
+      <c r="I687" t="n">
+        <v>107</v>
+      </c>
+      <c r="J687" t="n">
+        <v>3</v>
+      </c>
+      <c r="K687" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L687" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M687" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B688" t="n">
+        <v>523</v>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E688" t="n">
+        <v>23</v>
+      </c>
+      <c r="F688" t="n">
+        <v>29</v>
+      </c>
+      <c r="G688" t="n">
+        <v>24</v>
+      </c>
+      <c r="H688" t="n">
+        <v>26</v>
+      </c>
+      <c r="I688" t="n">
+        <v>102</v>
+      </c>
+      <c r="J688" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K688" t="n">
+        <v>211</v>
+      </c>
+      <c r="L688" t="n">
+        <v>220</v>
+      </c>
+      <c r="M688" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B689" t="n">
+        <v>524</v>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E689" t="n">
+        <v>34</v>
+      </c>
+      <c r="F689" t="n">
+        <v>35</v>
+      </c>
+      <c r="G689" t="n">
+        <v>36</v>
+      </c>
+      <c r="H689" t="n">
+        <v>19</v>
+      </c>
+      <c r="I689" t="n">
+        <v>124</v>
+      </c>
+      <c r="J689" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K689" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="L689" t="n">
+        <v>-260</v>
+      </c>
+      <c r="M689" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B690" t="n">
+        <v>525</v>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>Memphis</t>
+        </is>
+      </c>
+      <c r="E690" t="n">
+        <v>22</v>
+      </c>
+      <c r="F690" t="n">
+        <v>27</v>
+      </c>
+      <c r="G690" t="n">
+        <v>23</v>
+      </c>
+      <c r="H690" t="n">
+        <v>25</v>
+      </c>
+      <c r="I690" t="n">
+        <v>97</v>
+      </c>
+      <c r="J690" t="n">
+        <v>216.5</v>
+      </c>
+      <c r="K690" t="n">
+        <v>215</v>
+      </c>
+      <c r="L690" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M690" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B691" t="n">
+        <v>526</v>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E691" t="n">
+        <v>18</v>
+      </c>
+      <c r="F691" t="n">
+        <v>19</v>
+      </c>
+      <c r="G691" t="n">
+        <v>21</v>
+      </c>
+      <c r="H691" t="n">
+        <v>32</v>
+      </c>
+      <c r="I691" t="n">
+        <v>90</v>
+      </c>
+      <c r="J691" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K691" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L691" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M691" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B692" t="n">
+        <v>527</v>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>SanAntonio</t>
+        </is>
+      </c>
+      <c r="E692" t="n">
+        <v>36</v>
+      </c>
+      <c r="F692" t="n">
+        <v>31</v>
+      </c>
+      <c r="G692" t="n">
+        <v>32</v>
+      </c>
+      <c r="H692" t="n">
+        <v>13</v>
+      </c>
+      <c r="I692" t="n">
+        <v>112</v>
+      </c>
+      <c r="J692" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="K692" t="n">
+        <v>219</v>
+      </c>
+      <c r="L692" t="n">
+        <v>330</v>
+      </c>
+      <c r="M692" t="n">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B693" t="n">
+        <v>528</v>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>GoldenState</t>
+        </is>
+      </c>
+      <c r="E693" t="n">
+        <v>21</v>
+      </c>
+      <c r="F693" t="n">
+        <v>37</v>
+      </c>
+      <c r="G693" t="n">
+        <v>30</v>
+      </c>
+      <c r="H693" t="n">
+        <v>19</v>
+      </c>
+      <c r="I693" t="n">
+        <v>107</v>
+      </c>
+      <c r="J693" t="n">
+        <v>10</v>
+      </c>
+      <c r="K693" t="n">
+        <v>9</v>
+      </c>
+      <c r="L693" t="n">
+        <v>-400</v>
+      </c>
+      <c r="M693" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B694" t="n">
+        <v>529</v>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>Boston</t>
+        </is>
+      </c>
+      <c r="E694" t="n">
+        <v>38</v>
+      </c>
+      <c r="F694" t="n">
+        <v>26</v>
+      </c>
+      <c r="G694" t="n">
+        <v>39</v>
+      </c>
+      <c r="H694" t="n">
+        <v>42</v>
+      </c>
+      <c r="I694" t="n">
+        <v>145</v>
+      </c>
+      <c r="J694" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K694" t="n">
+        <v>211</v>
+      </c>
+      <c r="L694" t="n">
+        <v>-105</v>
+      </c>
+      <c r="M694" t="n">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B695" t="n">
+        <v>530</v>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>Portland</t>
+        </is>
+      </c>
+      <c r="E695" t="n">
+        <v>23</v>
+      </c>
+      <c r="F695" t="n">
+        <v>35</v>
+      </c>
+      <c r="G695" t="n">
+        <v>26</v>
+      </c>
+      <c r="H695" t="n">
+        <v>33</v>
+      </c>
+      <c r="I695" t="n">
+        <v>117</v>
+      </c>
+      <c r="J695" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="K695" t="n">
+        <v>1</v>
+      </c>
+      <c r="L695" t="n">
+        <v>-115</v>
+      </c>
+      <c r="M695" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B696" t="n">
+        <v>531</v>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E696" t="n">
+        <v>29</v>
+      </c>
+      <c r="F696" t="n">
+        <v>16</v>
+      </c>
+      <c r="G696" t="n">
+        <v>25</v>
+      </c>
+      <c r="H696" t="n">
+        <v>29</v>
+      </c>
+      <c r="I696" t="n">
+        <v>99</v>
+      </c>
+      <c r="J696" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K696" t="n">
+        <v>2</v>
+      </c>
+      <c r="L696" t="n">
+        <v>-125</v>
+      </c>
+      <c r="M696" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B697" t="n">
+        <v>532</v>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>Sacramento</t>
+        </is>
+      </c>
+      <c r="E697" t="n">
+        <v>29</v>
+      </c>
+      <c r="F697" t="n">
+        <v>21</v>
+      </c>
+      <c r="G697" t="n">
+        <v>26</v>
+      </c>
+      <c r="H697" t="n">
+        <v>28</v>
+      </c>
+      <c r="I697" t="n">
+        <v>104</v>
+      </c>
+      <c r="J697" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K697" t="n">
+        <v>219</v>
+      </c>
+      <c r="L697" t="n">
+        <v>105</v>
+      </c>
+      <c r="M697" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B698" t="n">
+        <v>533</v>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="E698" t="n">
+        <v>32</v>
+      </c>
+      <c r="F698" t="n">
+        <v>28</v>
+      </c>
+      <c r="G698" t="n">
+        <v>31</v>
+      </c>
+      <c r="H698" t="n">
+        <v>18</v>
+      </c>
+      <c r="I698" t="n">
+        <v>109</v>
+      </c>
+      <c r="J698" t="n">
+        <v>6</v>
+      </c>
+      <c r="K698" t="n">
+        <v>5</v>
+      </c>
+      <c r="L698" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M698" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B699" t="n">
+        <v>534</v>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E699" t="n">
+        <v>29</v>
+      </c>
+      <c r="F699" t="n">
+        <v>26</v>
+      </c>
+      <c r="G699" t="n">
+        <v>27</v>
+      </c>
+      <c r="H699" t="n">
+        <v>26</v>
+      </c>
+      <c r="I699" t="n">
+        <v>108</v>
+      </c>
+      <c r="J699" t="n">
+        <v>210</v>
+      </c>
+      <c r="K699" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="L699" t="n">
+        <v>175</v>
+      </c>
+      <c r="M699" t="n">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B700" t="n">
+        <v>535</v>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E700" t="n">
+        <v>12</v>
+      </c>
+      <c r="F700" t="n">
+        <v>30</v>
+      </c>
+      <c r="G700" t="n">
+        <v>26</v>
+      </c>
+      <c r="H700" t="n">
+        <v>22</v>
+      </c>
+      <c r="I700" t="n">
+        <v>90</v>
+      </c>
+      <c r="J700" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="K700" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="L700" t="n">
+        <v>100</v>
+      </c>
+      <c r="M700" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B701" t="n">
+        <v>536</v>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>Toronto</t>
+        </is>
+      </c>
+      <c r="E701" t="n">
+        <v>23</v>
+      </c>
+      <c r="F701" t="n">
+        <v>40</v>
+      </c>
+      <c r="G701" t="n">
+        <v>21</v>
+      </c>
+      <c r="H701" t="n">
+        <v>18</v>
+      </c>
+      <c r="I701" t="n">
+        <v>102</v>
+      </c>
+      <c r="J701" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K701" t="n">
+        <v>1</v>
+      </c>
+      <c r="L701" t="n">
+        <v>-120</v>
+      </c>
+      <c r="M701" t="n">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B702" t="n">
+        <v>537</v>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="E702" t="n">
+        <v>30</v>
+      </c>
+      <c r="F702" t="n">
+        <v>38</v>
+      </c>
+      <c r="G702" t="n">
+        <v>31</v>
+      </c>
+      <c r="H702" t="n">
+        <v>31</v>
+      </c>
+      <c r="I702" t="n">
+        <v>130</v>
+      </c>
+      <c r="J702" t="n">
+        <v>224.5</v>
+      </c>
+      <c r="K702" t="n">
+        <v>225.5</v>
+      </c>
+      <c r="L702" t="n">
+        <v>270</v>
+      </c>
+      <c r="M702" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B703" t="n">
+        <v>538</v>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E703" t="n">
+        <v>30</v>
+      </c>
+      <c r="F703" t="n">
+        <v>31</v>
+      </c>
+      <c r="G703" t="n">
+        <v>31</v>
+      </c>
+      <c r="H703" t="n">
+        <v>35</v>
+      </c>
+      <c r="I703" t="n">
+        <v>127</v>
+      </c>
+      <c r="J703" t="n">
+        <v>7</v>
+      </c>
+      <c r="K703" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L703" t="n">
+        <v>-330</v>
+      </c>
+      <c r="M703" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B704" t="n">
+        <v>539</v>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E704" t="n">
+        <v>26</v>
+      </c>
+      <c r="F704" t="n">
+        <v>23</v>
+      </c>
+      <c r="G704" t="n">
+        <v>36</v>
+      </c>
+      <c r="H704" t="n">
+        <v>23</v>
+      </c>
+      <c r="I704" t="n">
+        <v>108</v>
+      </c>
+      <c r="J704" t="n">
+        <v>3</v>
+      </c>
+      <c r="K704" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L704" t="n">
+        <v>-145</v>
+      </c>
+      <c r="M704" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B705" t="n">
+        <v>540</v>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E705" t="n">
+        <v>28</v>
+      </c>
+      <c r="F705" t="n">
+        <v>29</v>
+      </c>
+      <c r="G705" t="n">
+        <v>37</v>
+      </c>
+      <c r="H705" t="n">
+        <v>24</v>
+      </c>
+      <c r="I705" t="n">
+        <v>118</v>
+      </c>
+      <c r="J705" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="K705" t="n">
+        <v>222</v>
+      </c>
+      <c r="L705" t="n">
+        <v>125</v>
+      </c>
+      <c r="M705" t="n">
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B706" t="n">
+        <v>541</v>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E706" t="n">
+        <v>23</v>
+      </c>
+      <c r="F706" t="n">
+        <v>44</v>
+      </c>
+      <c r="G706" t="n">
+        <v>28</v>
+      </c>
+      <c r="H706" t="n">
+        <v>24</v>
+      </c>
+      <c r="I706" t="n">
+        <v>127</v>
+      </c>
+      <c r="J706" t="n">
+        <v>206.5</v>
+      </c>
+      <c r="K706" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L706" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M706" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B707" t="n">
+        <v>542</v>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="E707" t="n">
+        <v>34</v>
+      </c>
+      <c r="F707" t="n">
+        <v>28</v>
+      </c>
+      <c r="G707" t="n">
+        <v>31</v>
+      </c>
+      <c r="H707" t="n">
+        <v>26</v>
+      </c>
+      <c r="I707" t="n">
+        <v>124</v>
+      </c>
+      <c r="J707" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K707" t="n">
+        <v>214</v>
+      </c>
+      <c r="L707" t="n">
+        <v>250</v>
+      </c>
+      <c r="M707" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B708" t="n">
+        <v>543</v>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>OklahomaCity</t>
+        </is>
+      </c>
+      <c r="E708" t="n">
+        <v>28</v>
+      </c>
+      <c r="F708" t="n">
+        <v>22</v>
+      </c>
+      <c r="G708" t="n">
+        <v>22</v>
+      </c>
+      <c r="H708" t="n">
+        <v>42</v>
+      </c>
+      <c r="I708" t="n">
+        <v>114</v>
+      </c>
+      <c r="J708" t="n">
+        <v>206.5</v>
+      </c>
+      <c r="K708" t="n">
+        <v>205</v>
+      </c>
+      <c r="L708" t="n">
+        <v>135</v>
+      </c>
+      <c r="M708" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B709" t="n">
+        <v>544</v>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E709" t="n">
+        <v>37</v>
+      </c>
+      <c r="F709" t="n">
+        <v>26</v>
+      </c>
+      <c r="G709" t="n">
+        <v>18</v>
+      </c>
+      <c r="H709" t="n">
+        <v>22</v>
+      </c>
+      <c r="I709" t="n">
+        <v>103</v>
+      </c>
+      <c r="J709" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K709" t="n">
+        <v>3</v>
+      </c>
+      <c r="L709" t="n">
+        <v>-155</v>
+      </c>
+      <c r="M709" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B710" t="n">
+        <v>545</v>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E710" t="n">
+        <v>18</v>
+      </c>
+      <c r="F710" t="n">
+        <v>29</v>
+      </c>
+      <c r="G710" t="n">
+        <v>31</v>
+      </c>
+      <c r="H710" t="n">
+        <v>32</v>
+      </c>
+      <c r="I710" t="n">
+        <v>110</v>
+      </c>
+      <c r="J710" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="K710" t="n">
+        <v>211.5</v>
+      </c>
+      <c r="L710" t="n">
+        <v>190</v>
+      </c>
+      <c r="M710" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B711" t="n">
+        <v>546</v>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="E711" t="n">
+        <v>28</v>
+      </c>
+      <c r="F711" t="n">
+        <v>30</v>
+      </c>
+      <c r="G711" t="n">
+        <v>30</v>
+      </c>
+      <c r="H711" t="n">
+        <v>28</v>
+      </c>
+      <c r="I711" t="n">
+        <v>116</v>
+      </c>
+      <c r="J711" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K711" t="n">
+        <v>6</v>
+      </c>
+      <c r="L711" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M711" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B712" t="n">
+        <v>547</v>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>Memphis</t>
+        </is>
+      </c>
+      <c r="E712" t="n">
+        <v>34</v>
+      </c>
+      <c r="F712" t="n">
+        <v>26</v>
+      </c>
+      <c r="G712" t="n">
+        <v>22</v>
+      </c>
+      <c r="H712" t="n">
+        <v>23</v>
+      </c>
+      <c r="I712" t="n">
+        <v>105</v>
+      </c>
+      <c r="J712" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K712" t="n">
+        <v>213</v>
+      </c>
+      <c r="L712" t="n">
+        <v>185</v>
+      </c>
+      <c r="M712" t="n">
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B713" t="n">
+        <v>548</v>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E713" t="n">
+        <v>25</v>
+      </c>
+      <c r="F713" t="n">
+        <v>24</v>
+      </c>
+      <c r="G713" t="n">
+        <v>18</v>
+      </c>
+      <c r="H713" t="n">
+        <v>23</v>
+      </c>
+      <c r="I713" t="n">
+        <v>90</v>
+      </c>
+      <c r="J713" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K713" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L713" t="n">
+        <v>-215</v>
+      </c>
+      <c r="M713" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B714" t="n">
+        <v>549</v>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E714" t="n">
+        <v>27</v>
+      </c>
+      <c r="F714" t="n">
+        <v>22</v>
+      </c>
+      <c r="G714" t="n">
+        <v>22</v>
+      </c>
+      <c r="H714" t="n">
+        <v>26</v>
+      </c>
+      <c r="I714" t="n">
+        <v>97</v>
+      </c>
+      <c r="J714" t="n">
+        <v>214</v>
+      </c>
+      <c r="K714" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="L714" t="n">
+        <v>115</v>
+      </c>
+      <c r="M714" t="n">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B715" t="n">
+        <v>550</v>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E715" t="n">
+        <v>18</v>
+      </c>
+      <c r="F715" t="n">
+        <v>28</v>
+      </c>
+      <c r="G715" t="n">
+        <v>31</v>
+      </c>
+      <c r="H715" t="n">
+        <v>32</v>
+      </c>
+      <c r="I715" t="n">
+        <v>109</v>
+      </c>
+      <c r="J715" t="n">
+        <v>5</v>
+      </c>
+      <c r="K715" t="n">
+        <v>2</v>
+      </c>
+      <c r="L715" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M715" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B716" t="n">
+        <v>551</v>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E716" t="n">
+        <v>33</v>
+      </c>
+      <c r="F716" t="n">
+        <v>28</v>
+      </c>
+      <c r="G716" t="n">
+        <v>35</v>
+      </c>
+      <c r="H716" t="n">
+        <v>25</v>
+      </c>
+      <c r="I716" t="n">
+        <v>121</v>
+      </c>
+      <c r="J716" t="n">
+        <v>219.5</v>
+      </c>
+      <c r="K716" t="n">
+        <v>221.5</v>
+      </c>
+      <c r="L716" t="n">
+        <v>110</v>
+      </c>
+      <c r="M716" t="n">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B717" t="n">
+        <v>552</v>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E717" t="n">
+        <v>24</v>
+      </c>
+      <c r="F717" t="n">
+        <v>24</v>
+      </c>
+      <c r="G717" t="n">
+        <v>30</v>
+      </c>
+      <c r="H717" t="n">
+        <v>32</v>
+      </c>
+      <c r="I717" t="n">
+        <v>110</v>
+      </c>
+      <c r="J717" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K717" t="n">
+        <v>2</v>
+      </c>
+      <c r="L717" t="n">
+        <v>-130</v>
+      </c>
+      <c r="M717" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B718" t="n">
+        <v>553</v>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E718" t="n">
+        <v>24</v>
+      </c>
+      <c r="F718" t="n">
+        <v>26</v>
+      </c>
+      <c r="G718" t="n">
+        <v>28</v>
+      </c>
+      <c r="H718" t="n">
+        <v>26</v>
+      </c>
+      <c r="I718" t="n">
+        <v>104</v>
+      </c>
+      <c r="J718" t="n">
+        <v>213.5</v>
+      </c>
+      <c r="K718" t="n">
+        <v>215</v>
+      </c>
+      <c r="L718" t="n">
+        <v>300</v>
+      </c>
+      <c r="M718" t="n">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B719" t="n">
+        <v>554</v>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>Milwaukee</t>
+        </is>
+      </c>
+      <c r="E719" t="n">
+        <v>24</v>
+      </c>
+      <c r="F719" t="n">
+        <v>32</v>
+      </c>
+      <c r="G719" t="n">
+        <v>32</v>
+      </c>
+      <c r="H719" t="n">
+        <v>24</v>
+      </c>
+      <c r="I719" t="n">
+        <v>112</v>
+      </c>
+      <c r="J719" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K719" t="n">
+        <v>9</v>
+      </c>
+      <c r="L719" t="n">
+        <v>-360</v>
+      </c>
+      <c r="M719" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B720" t="n">
+        <v>555</v>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>SanAntonio</t>
+        </is>
+      </c>
+      <c r="E720" t="n">
+        <v>33</v>
+      </c>
+      <c r="F720" t="n">
+        <v>15</v>
+      </c>
+      <c r="G720" t="n">
+        <v>22</v>
+      </c>
+      <c r="H720" t="n">
+        <v>34</v>
+      </c>
+      <c r="I720" t="n">
+        <v>104</v>
+      </c>
+      <c r="J720" t="n">
+        <v>218.5</v>
+      </c>
+      <c r="K720" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="L720" t="n">
+        <v>250</v>
+      </c>
+      <c r="M720" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B721" t="n">
+        <v>556</v>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>Phoenix</t>
+        </is>
+      </c>
+      <c r="E721" t="n">
+        <v>26</v>
+      </c>
+      <c r="F721" t="n">
+        <v>25</v>
+      </c>
+      <c r="G721" t="n">
+        <v>28</v>
+      </c>
+      <c r="H721" t="n">
+        <v>29</v>
+      </c>
+      <c r="I721" t="n">
+        <v>108</v>
+      </c>
+      <c r="J721" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K721" t="n">
+        <v>7</v>
+      </c>
+      <c r="L721" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M721" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B722" t="n">
+        <v>557</v>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>LAClippers</t>
+        </is>
+      </c>
+      <c r="E722" t="n">
+        <v>27</v>
+      </c>
+      <c r="F722" t="n">
+        <v>21</v>
+      </c>
+      <c r="G722" t="n">
+        <v>29</v>
+      </c>
+      <c r="H722" t="n">
+        <v>25</v>
+      </c>
+      <c r="I722" t="n">
+        <v>102</v>
+      </c>
+      <c r="J722" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K722" t="n">
+        <v>5</v>
+      </c>
+      <c r="L722" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M722" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B723" t="n">
+        <v>558</v>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>Portland</t>
+        </is>
+      </c>
+      <c r="E723" t="n">
+        <v>26</v>
+      </c>
+      <c r="F723" t="n">
+        <v>23</v>
+      </c>
+      <c r="G723" t="n">
+        <v>25</v>
+      </c>
+      <c r="H723" t="n">
+        <v>16</v>
+      </c>
+      <c r="I723" t="n">
+        <v>90</v>
+      </c>
+      <c r="J723" t="n">
+        <v>215.5</v>
+      </c>
+      <c r="K723" t="n">
+        <v>213</v>
+      </c>
+      <c r="L723" t="n">
+        <v>175</v>
+      </c>
+      <c r="M723" t="n">
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B724" t="n">
+        <v>559</v>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="E724" t="n">
+        <v>26</v>
+      </c>
+      <c r="F724" t="n">
+        <v>18</v>
+      </c>
+      <c r="G724" t="n">
+        <v>35</v>
+      </c>
+      <c r="H724" t="n">
+        <v>16</v>
+      </c>
+      <c r="I724" t="n">
+        <v>95</v>
+      </c>
+      <c r="J724" t="n">
+        <v>216</v>
+      </c>
+      <c r="K724" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="L724" t="n">
+        <v>950</v>
+      </c>
+      <c r="M724" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B725" t="n">
+        <v>560</v>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>GoldenState</t>
+        </is>
+      </c>
+      <c r="E725" t="n">
+        <v>31</v>
+      </c>
+      <c r="F725" t="n">
+        <v>34</v>
+      </c>
+      <c r="G725" t="n">
+        <v>33</v>
+      </c>
+      <c r="H725" t="n">
+        <v>28</v>
+      </c>
+      <c r="I725" t="n">
+        <v>126</v>
+      </c>
+      <c r="J725" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="K725" t="n">
+        <v>16</v>
+      </c>
+      <c r="L725" t="n">
+        <v>-1800</v>
+      </c>
+      <c r="M725" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>